<commit_message>
I snuck in the use of com.google.collect.Range instead of either making a new predicate that took the low/high bounds or two predicates (one for greater than and one for less than) joined by and.
</commit_message>
<xml_diff>
--- a/Chilis.xlsx
+++ b/Chilis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19065" windowHeight="6135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19065" windowHeight="6135" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="180">
   <si>
     <t>Name</t>
   </si>
@@ -917,7 +917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B100" workbookViewId="0">
       <selection activeCell="R1" sqref="R1:U3"/>
     </sheetView>
   </sheetViews>
@@ -8324,10 +8324,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8335,7 +8335,7 @@
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>177</v>
       </c>
@@ -8351,8 +8351,23 @@
       <c r="E1">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1">
+        <v>45</v>
+      </c>
+      <c r="G1">
+        <v>50</v>
+      </c>
+      <c r="H1">
+        <v>55</v>
+      </c>
+      <c r="I1">
+        <v>60</v>
+      </c>
+      <c r="J1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>178</v>
       </c>
@@ -8372,8 +8387,28 @@
         <f>COUNTIF(Sheet1!$P$2:$P$164,"&lt;" &amp; E1)</f>
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>COUNTIF(Sheet1!$P$2:$P$164,"&lt;" &amp; F1)</f>
+        <v>67</v>
+      </c>
+      <c r="G2">
+        <f>COUNTIF(Sheet1!$P$2:$P$164,"&lt;" &amp; G1)</f>
+        <v>96</v>
+      </c>
+      <c r="H2">
+        <f>COUNTIF(Sheet1!$P$2:$P$164,"&lt;" &amp; H1)</f>
+        <v>123</v>
+      </c>
+      <c r="I2">
+        <f>COUNTIF(Sheet1!$P$2:$P$164,"&lt;" &amp; I1)</f>
+        <v>139</v>
+      </c>
+      <c r="J2">
+        <f>COUNTIF(Sheet1!$P$2:$P$164,"&lt;" &amp; J1)</f>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -8393,8 +8428,193 @@
         <f>COUNTIFS(Sheet1!$P$2:$P$164,"&gt;0",Sheet1!$P$2:$P$164,"&lt;"&amp;E1)</f>
         <v>32</v>
       </c>
+      <c r="F3" s="1">
+        <f>COUNTIFS(Sheet1!$P$2:$P$164,"&gt;0",Sheet1!$P$2:$P$164,"&lt;"&amp;F1)</f>
+        <v>53</v>
+      </c>
+      <c r="G3" s="1">
+        <f>COUNTIFS(Sheet1!$P$2:$P$164,"&gt;0",Sheet1!$P$2:$P$164,"&lt;"&amp;G1)</f>
+        <v>82</v>
+      </c>
+      <c r="H3" s="1">
+        <f>COUNTIFS(Sheet1!$P$2:$P$164,"&gt;0",Sheet1!$P$2:$P$164,"&lt;"&amp;H1)</f>
+        <v>109</v>
+      </c>
+      <c r="I3" s="1">
+        <f>COUNTIFS(Sheet1!$P$2:$P$164,"&gt;0",Sheet1!$P$2:$P$164,"&lt;"&amp;I1)</f>
+        <v>125</v>
+      </c>
+      <c r="J3" s="1">
+        <f>COUNTIFS(Sheet1!$P$2:$P$164,"&gt;0",Sheet1!$P$2:$P$164,"&lt;"&amp;J1)</f>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A4,Sheet1!$P$2:$P$164,"&lt;"&amp;B$1)</f>
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A4,Sheet1!$P$2:$P$164,"&lt;"&amp;C$1)</f>
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A4,Sheet1!$P$2:$P$164,"&lt;"&amp;D$1)</f>
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A4,Sheet1!$P$2:$P$164,"&lt;"&amp;E$1)</f>
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A4,Sheet1!$P$2:$P$164,"&lt;"&amp;F$1)</f>
+        <v>26</v>
+      </c>
+      <c r="G4">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A4,Sheet1!$P$2:$P$164,"&lt;"&amp;G$1)</f>
+        <v>40</v>
+      </c>
+      <c r="H4">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A4,Sheet1!$P$2:$P$164,"&lt;"&amp;H$1)</f>
+        <v>53</v>
+      </c>
+      <c r="I4">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A4,Sheet1!$P$2:$P$164,"&lt;"&amp;I$1)</f>
+        <v>55</v>
+      </c>
+      <c r="J4">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A4,Sheet1!$P$2:$P$164,"&lt;"&amp;J$1)</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A5,Sheet1!$P$2:$P$164,"&lt;"&amp;B$1)</f>
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A5,Sheet1!$P$2:$P$164,"&lt;"&amp;C$1)</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A5,Sheet1!$P$2:$P$164,"&lt;"&amp;D$1)</f>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A5,Sheet1!$P$2:$P$164,"&lt;"&amp;E$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A5,Sheet1!$P$2:$P$164,"&lt;"&amp;F$1)</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A5,Sheet1!$P$2:$P$164,"&lt;"&amp;G$1)</f>
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A5,Sheet1!$P$2:$P$164,"&lt;"&amp;H$1)</f>
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A5,Sheet1!$P$2:$P$164,"&lt;"&amp;I$1)</f>
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A5,Sheet1!$P$2:$P$164,"&lt;"&amp;J$1)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A6,Sheet1!$P$2:$P$164,"&lt;"&amp;B$1)</f>
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A6,Sheet1!$P$2:$P$164,"&lt;"&amp;C$1)</f>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A6,Sheet1!$P$2:$P$164,"&lt;"&amp;D$1)</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A6,Sheet1!$P$2:$P$164,"&lt;"&amp;E$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A6,Sheet1!$P$2:$P$164,"&lt;"&amp;F$1)</f>
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A6,Sheet1!$P$2:$P$164,"&lt;"&amp;G$1)</f>
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A6,Sheet1!$P$2:$P$164,"&lt;"&amp;H$1)</f>
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A6,Sheet1!$P$2:$P$164,"&lt;"&amp;I$1)</f>
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A6,Sheet1!$P$2:$P$164,"&lt;"&amp;J$1)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A7,Sheet1!$P$2:$P$164,"&lt;"&amp;B$1)</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A7,Sheet1!$P$2:$P$164,"&lt;"&amp;C$1)</f>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A7,Sheet1!$P$2:$P$164,"&lt;"&amp;D$1)</f>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A7,Sheet1!$P$2:$P$164,"&lt;"&amp;E$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A7,Sheet1!$P$2:$P$164,"&lt;"&amp;F$1)</f>
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A7,Sheet1!$P$2:$P$164,"&lt;"&amp;G$1)</f>
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A7,Sheet1!$P$2:$P$164,"&lt;"&amp;H$1)</f>
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A7,Sheet1!$P$2:$P$164,"&lt;"&amp;I$1)</f>
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <f>COUNTIFS(Sheet1!$N$2:$N$164,"=" &amp; $A7,Sheet1!$P$2:$P$164,"&lt;"&amp;J$1)</f>
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>